<commit_message>
added batch mode training
</commit_message>
<xml_diff>
--- a/results/KerasTraining.xlsx
+++ b/results/KerasTraining.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31575" windowHeight="10170" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="31575" windowHeight="10170"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="258">
   <si>
     <t>loss: 3.0443e-04 - mean_squared_error: 3.0443e-04 - mean_absolute_error: 0.0080</t>
   </si>
@@ -731,6 +731,81 @@
   </si>
   <si>
     <t>Inference time (GPU):  3.8418056964874268  seconds</t>
+  </si>
+  <si>
+    <t>xxxxxxxx</t>
+  </si>
+  <si>
+    <t>Long runs</t>
+  </si>
+  <si>
+    <t>batch 115216 7201x7201 data</t>
+  </si>
+  <si>
+    <t>epoch 1000</t>
+  </si>
+  <si>
+    <t>loss: 3.2716e-06 - mean_squared_error: 3.2716e-06 - mean_absolute_error: 3.3996e-04</t>
+  </si>
+  <si>
+    <t>Training time  28130.3430352211  seconds</t>
+  </si>
+  <si>
+    <t>CBar error =  89.67707550837889  CBarObs= 12.497717170746977  CBarPred= 102.17479267912587</t>
+  </si>
+  <si>
+    <t>Inference time:  1013.4813346862793  seconds</t>
+  </si>
+  <si>
+    <t>Training time  7968.715792894363  seconds</t>
+  </si>
+  <si>
+    <t>for 200 epoch with full data, 28804 batch</t>
+  </si>
+  <si>
+    <t>batch 230432</t>
+  </si>
+  <si>
+    <t>CBar error =  89.70095302374934  CBarObs= 12.497717170746977  CBarPred= 102.19867019449632</t>
+  </si>
+  <si>
+    <t>Inference time:  0.9794225692749023  seconds</t>
+  </si>
+  <si>
+    <t>loss: 2.9593e-06 - mean_squared_error: 2.9593e-06 - mean_absolute_error: 3.7637e-04</t>
+  </si>
+  <si>
+    <t>maxOi= 36393.0 maxDj= 6153.0 maxCij= 656.0 maxTij= 2270.0</t>
+  </si>
+  <si>
+    <t>scaleOiDj= 2.1982249333663068e-05 scaleCij= 0.0012195121951219512 scaleTij= 0.0003524229074889868</t>
+  </si>
+  <si>
+    <t>100 epoch</t>
+  </si>
+  <si>
+    <t>loss: 2.9404e-06 - mean_squared_error: 2.9404e-06 - mean_absolute_error: 3.8107e-04</t>
+  </si>
+  <si>
+    <t>Training time  2650.5804274082184  seconds</t>
+  </si>
+  <si>
+    <t>CBar error =  86.15846624851491  CBarObs= 12.497717170746977  CBarPred= 98.6561834192619</t>
+  </si>
+  <si>
+    <t>Inference time:  0.9164769649505615  seconds</t>
+  </si>
+  <si>
+    <t>loss: 2.9233e-06 - mean_squared_error: 2.9233e-06 - mean_absolute_error: 3.8310e-04</t>
+  </si>
+  <si>
+    <t>Training time  2639.9246554374695  seconds</t>
+  </si>
+  <si>
+    <t>CBar error =  85.79124932033587  CBarObs= 12.497717170746977  CBarPred= 98.28896649108285</t>
+  </si>
+  <si>
+    <t>Inference time:  0.9934592247009277  seconds</t>
   </si>
 </sst>
 </file>
@@ -832,7 +907,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1742,7 +1816,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1865,7 +1938,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2923,10 +2995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H350"/>
+  <dimension ref="A1:H381"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A340" workbookViewId="0">
+      <selection activeCell="A382" sqref="A382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4245,6 +4317,134 @@
     <row r="350" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>219</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>241</v>
+      </c>
+      <c r="F365" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -6699,7 +6899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Z37" sqref="Z37"/>
     </sheetView>
   </sheetViews>

</xml_diff>